<commit_message>
Tenure Self Run without creation
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Leave_Scenarios_Without_Creation.xlsx
+++ b/src/main/resources/TestData/Leave_Scenarios_Without_Creation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="All_without_Creation" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet6" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Tenure_without_Creation!$A$1:$Y$83</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">All_Without_Probation!$A$1:$U$83</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -5404,6 +5405,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -5411,13 +5416,15 @@
   </sheetPr>
   <dimension ref="A1:U247"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21488,20 +21495,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21581,7 +21588,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -21589,7 +21596,7 @@
         <v>522</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>523</v>
@@ -21658,7 +21665,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -21666,7 +21673,7 @@
         <v>527</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>528</v>
@@ -21735,7 +21742,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -21743,7 +21750,7 @@
         <v>529</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>530</v>
@@ -21812,7 +21819,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -21820,7 +21827,7 @@
         <v>531</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>532</v>
@@ -21889,7 +21896,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -21897,7 +21904,7 @@
         <v>533</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>534</v>
@@ -21966,7 +21973,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -21974,7 +21981,7 @@
         <v>535</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>536</v>
@@ -22043,7 +22050,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -22051,7 +22058,7 @@
         <v>537</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>538</v>
@@ -22120,7 +22127,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -22128,7 +22135,7 @@
         <v>539</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>540</v>
@@ -22197,7 +22204,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -22205,7 +22212,7 @@
         <v>541</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>542</v>
@@ -22274,7 +22281,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -22282,7 +22289,7 @@
         <v>543</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>544</v>
@@ -22351,7 +22358,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -22359,7 +22366,7 @@
         <v>545</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>546</v>
@@ -22428,7 +22435,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
@@ -22436,7 +22443,7 @@
         <v>547</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>548</v>
@@ -22505,7 +22512,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
@@ -22513,7 +22520,7 @@
         <v>549</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>550</v>
@@ -22590,7 +22597,7 @@
         <v>551</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>552</v>
@@ -22659,7 +22666,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -22667,7 +22674,7 @@
         <v>553</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>554</v>
@@ -22736,7 +22743,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -22744,7 +22751,7 @@
         <v>555</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>556</v>
@@ -22813,7 +22820,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -22821,7 +22828,7 @@
         <v>557</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>558</v>
@@ -22890,7 +22897,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -22898,7 +22905,7 @@
         <v>559</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>560</v>
@@ -23044,7 +23051,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -23052,7 +23059,7 @@
         <v>563</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>564</v>
@@ -23121,7 +23128,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -23129,7 +23136,7 @@
         <v>565</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>566</v>
@@ -23198,7 +23205,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -23206,7 +23213,7 @@
         <v>567</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>568</v>
@@ -23275,7 +23282,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -23283,7 +23290,7 @@
         <v>569</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>570</v>
@@ -23429,7 +23436,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
@@ -23437,7 +23444,7 @@
         <v>573</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>574</v>
@@ -23506,7 +23513,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>21</v>
       </c>
@@ -23514,7 +23521,7 @@
         <v>575</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>576</v>
@@ -23583,7 +23590,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
@@ -23591,7 +23598,7 @@
         <v>577</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>578</v>
@@ -23660,7 +23667,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
         <v>21</v>
       </c>
@@ -23668,7 +23675,7 @@
         <v>579</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>580</v>
@@ -23745,7 +23752,7 @@
         <v>581</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>582</v>
@@ -23814,7 +23821,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>21</v>
       </c>
@@ -23822,7 +23829,7 @@
         <v>583</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>584</v>
@@ -23891,7 +23898,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
@@ -23899,7 +23906,7 @@
         <v>585</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>586</v>
@@ -23968,7 +23975,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
@@ -23976,7 +23983,7 @@
         <v>587</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>588</v>
@@ -24045,7 +24052,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>21</v>
       </c>
@@ -24053,7 +24060,7 @@
         <v>589</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>590</v>
@@ -24122,7 +24129,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>21</v>
       </c>
@@ -24130,7 +24137,7 @@
         <v>591</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>592</v>
@@ -24199,7 +24206,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>21</v>
       </c>
@@ -24207,7 +24214,7 @@
         <v>593</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>594</v>
@@ -24276,7 +24283,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
@@ -24284,7 +24291,7 @@
         <v>595</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>596</v>
@@ -24353,7 +24360,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>21</v>
       </c>
@@ -24361,7 +24368,7 @@
         <v>597</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>598</v>
@@ -24430,7 +24437,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
@@ -24438,7 +24445,7 @@
         <v>599</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>600</v>
@@ -24507,7 +24514,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
@@ -24515,7 +24522,7 @@
         <v>601</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>602</v>
@@ -24584,7 +24591,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
         <v>21</v>
       </c>
@@ -24592,7 +24599,7 @@
         <v>603</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>604</v>
@@ -24661,7 +24668,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
         <v>21</v>
       </c>
@@ -24669,7 +24676,7 @@
         <v>605</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>606</v>
@@ -24738,7 +24745,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="113.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>21</v>
       </c>
@@ -24746,7 +24753,7 @@
         <v>607</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>608</v>
@@ -24815,7 +24822,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="s">
         <v>21</v>
       </c>
@@ -24823,7 +24830,7 @@
         <v>609</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>610</v>
@@ -24892,7 +24899,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
         <v>21</v>
       </c>
@@ -24900,7 +24907,7 @@
         <v>611</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>612</v>
@@ -24969,7 +24976,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="147" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
         <v>21</v>
       </c>
@@ -24977,7 +24984,7 @@
         <v>613</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>614</v>
@@ -25046,7 +25053,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="s">
         <v>21</v>
       </c>
@@ -25054,7 +25061,7 @@
         <v>615</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>616</v>
@@ -25123,7 +25130,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="s">
         <v>21</v>
       </c>
@@ -25131,7 +25138,7 @@
         <v>617</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>618</v>
@@ -25200,7 +25207,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>21</v>
       </c>
@@ -25208,7 +25215,7 @@
         <v>619</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>620</v>
@@ -25277,7 +25284,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
@@ -25285,7 +25292,7 @@
         <v>621</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>622</v>
@@ -25354,7 +25361,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="s">
         <v>21</v>
       </c>
@@ -25362,7 +25369,7 @@
         <v>623</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>624</v>
@@ -25431,7 +25438,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="135.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
         <v>21</v>
       </c>
@@ -25439,7 +25446,7 @@
         <v>625</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>626</v>
@@ -25508,7 +25515,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="124.6" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
         <v>21</v>
       </c>
@@ -25516,7 +25523,7 @@
         <v>627</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>628</v>
@@ -25585,7 +25592,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
         <v>21</v>
       </c>
@@ -25593,7 +25600,7 @@
         <v>629</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>630</v>
@@ -25662,7 +25669,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
         <v>21</v>
       </c>
@@ -25670,7 +25677,7 @@
         <v>631</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>632</v>
@@ -25739,7 +25746,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="s">
         <v>21</v>
       </c>
@@ -25747,7 +25754,7 @@
         <v>633</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>634</v>
@@ -25816,7 +25823,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
         <v>21</v>
       </c>
@@ -25824,7 +25831,7 @@
         <v>635</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>636</v>
@@ -25893,7 +25900,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
         <v>21</v>
       </c>
@@ -25901,7 +25908,7 @@
         <v>637</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>638</v>
@@ -25970,7 +25977,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
         <v>21</v>
       </c>
@@ -25978,7 +25985,7 @@
         <v>639</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>640</v>
@@ -26047,7 +26054,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
         <v>21</v>
       </c>
@@ -26055,7 +26062,7 @@
         <v>641</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>642</v>
@@ -26124,7 +26131,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
         <v>21</v>
       </c>
@@ -26132,7 +26139,7 @@
         <v>643</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>644</v>
@@ -26201,7 +26208,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="s">
         <v>21</v>
       </c>
@@ -26209,7 +26216,7 @@
         <v>645</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>646</v>
@@ -26278,7 +26285,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="s">
         <v>21</v>
       </c>
@@ -26286,7 +26293,7 @@
         <v>647</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>648</v>
@@ -26355,7 +26362,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="s">
         <v>21</v>
       </c>
@@ -26363,7 +26370,7 @@
         <v>649</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>650</v>
@@ -26432,7 +26439,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="s">
         <v>21</v>
       </c>
@@ -26440,7 +26447,7 @@
         <v>651</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>652</v>
@@ -26509,7 +26516,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="s">
         <v>21</v>
       </c>
@@ -26517,7 +26524,7 @@
         <v>653</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>654</v>
@@ -26586,7 +26593,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="s">
         <v>21</v>
       </c>
@@ -26594,7 +26601,7 @@
         <v>655</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>656</v>
@@ -26663,7 +26670,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="158.2" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="s">
         <v>21</v>
       </c>
@@ -26671,7 +26678,7 @@
         <v>657</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>658</v>
@@ -26740,7 +26747,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="s">
         <v>21</v>
       </c>
@@ -26748,7 +26755,7 @@
         <v>659</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>660</v>
@@ -26817,7 +26824,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="s">
         <v>21</v>
       </c>
@@ -26825,7 +26832,7 @@
         <v>661</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>662</v>
@@ -26894,7 +26901,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="s">
         <v>21</v>
       </c>
@@ -26902,7 +26909,7 @@
         <v>663</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>664</v>
@@ -26971,7 +26978,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="s">
         <v>21</v>
       </c>
@@ -26979,7 +26986,7 @@
         <v>665</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>666</v>
@@ -27048,7 +27055,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="s">
         <v>21</v>
       </c>
@@ -27056,7 +27063,7 @@
         <v>667</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>668</v>
@@ -27125,7 +27132,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="s">
         <v>21</v>
       </c>
@@ -27133,7 +27140,7 @@
         <v>669</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>670</v>
@@ -27202,7 +27209,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
         <v>21</v>
       </c>
@@ -27210,7 +27217,7 @@
         <v>671</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>672</v>
@@ -27279,7 +27286,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
         <v>21</v>
       </c>
@@ -27287,7 +27294,7 @@
         <v>673</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>674</v>
@@ -27356,7 +27363,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
         <v>21</v>
       </c>
@@ -27364,7 +27371,7 @@
         <v>675</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>676</v>
@@ -27433,7 +27440,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
         <v>21</v>
       </c>
@@ -27441,7 +27448,7 @@
         <v>677</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>678</v>
@@ -27510,7 +27517,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -27518,7 +27525,7 @@
         <v>679</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>680</v>
@@ -27587,7 +27594,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
         <v>21</v>
       </c>
@@ -27595,7 +27602,7 @@
         <v>681</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>682</v>
@@ -27664,7 +27671,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
         <v>21</v>
       </c>
@@ -27672,7 +27679,7 @@
         <v>683</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>684</v>
@@ -27741,7 +27748,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="180.55" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
         <v>21</v>
       </c>
@@ -27749,7 +27756,7 @@
         <v>685</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>686</v>
@@ -27818,7 +27825,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="169.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="s">
         <v>21</v>
       </c>
@@ -27826,7 +27833,7 @@
         <v>687</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>688</v>
@@ -27896,6 +27903,28 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Y83">
+    <filterColumn colId="17">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Yes"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Yes"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Calendar Year"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="19">
+      <customFilters and="true">
+        <customFilter operator="equal" val="Yes"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -27903,6 +27932,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27919,13 +27949,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="4" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33349,13 +33377,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="4" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38777,9 +38803,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -44201,13 +44225,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="4" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="4" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="4" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="4" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57819,7 +57841,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>